<commit_message>
Added to markov models
time homogenous search for solutions 1 through 10 classes. Created excel matrices for 4 and 6
</commit_message>
<xml_diff>
--- a/R/complete8StatesCondProb.xlsx
+++ b/R/complete8StatesCondProb.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5481982-5392-4371-94CC-7D28F0BEEBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F98A32-096C-46FC-A21C-2BC92618ADD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$N$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -211,7 +211,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 1</c:v>
+                  <c:v>State 8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -280,43 +280,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2.2047684234645749E-2</c:v>
+                  <c:v>9.9999999999321573E-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3046972424085569E-2</c:v>
+                  <c:v>0.7016265604056392</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0629114033052673E-2</c:v>
+                  <c:v>0.42442550141671692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.890445842796287E-3</c:v>
+                  <c:v>0.45728933537503152</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2251178363368572</c:v>
+                  <c:v>9.3852416398575028E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0253851422455973E-2</c:v>
+                  <c:v>0.35407924289997772</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.2563427158311944E-3</c:v>
+                  <c:v>4.6142408067212128E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.999999999810545E-11</c:v>
+                  <c:v>0.77757230967003532</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.74584821953227221</c:v>
+                  <c:v>4.9356090172584577E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7907677807776448E-2</c:v>
+                  <c:v>0.89260979170291921</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2218930660137203</c:v>
+                  <c:v>0.74065643991960151</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.2385023482237487E-2</c:v>
+                  <c:v>0.99755492546134183</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.60238862898699674</c:v>
+                  <c:v>0.5692203845545537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,7 +336,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 2</c:v>
+                  <c:v>State 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -405,43 +405,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.21726863326839521</c:v>
+                  <c:v>5.2625069243399797E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2799956205332547E-2</c:v>
+                  <c:v>0.1583387228885309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8765374118686108E-2</c:v>
+                  <c:v>3.2360558366148671E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.860521497585321E-3</c:v>
+                  <c:v>0.42079215933093977</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5165162606031692E-3</c:v>
+                  <c:v>2.2122018740809969E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3155059660385122E-2</c:v>
+                  <c:v>2.0676260903289369E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.9999999990087394E-11</c:v>
+                  <c:v>9.999999999920666E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4262896519754919</c:v>
+                  <c:v>0.3095388591764453</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6531237197536032E-2</c:v>
+                  <c:v>8.9074146891717845E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9064631494888829E-3</c:v>
+                  <c:v>0.51097211206557314</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9999999992495097E-11</c:v>
+                  <c:v>2.8331160920852388E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.15455729869780421</c:v>
+                  <c:v>0.84011446552460134</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.14965503018695939</c:v>
+                  <c:v>0.27125329754273608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,7 +461,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 3</c:v>
+                  <c:v>State 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,43 +530,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.54070007486828675</c:v>
+                  <c:v>1.0735624609932321E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5407104201901702E-2</c:v>
+                  <c:v>4.4113077583493553E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74504643821964256</c:v>
+                  <c:v>4.1054355745552197E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.354811901022903</c:v>
+                  <c:v>0.1575702728459232</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1161355908351684</c:v>
+                  <c:v>1.673966584248299E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1395758925812996</c:v>
+                  <c:v>0.60610067961852132</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.4365109338377222E-2</c:v>
+                  <c:v>0.60385173341770948</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5199893524897879E-2</c:v>
+                  <c:v>5.0847866992160817E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1207850320130895</c:v>
+                  <c:v>1.5846966214778949E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6916553455223549E-3</c:v>
+                  <c:v>5.2494510671060764E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.81366235053645242</c:v>
+                  <c:v>3.496587641206412E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.63731989643767506</c:v>
+                  <c:v>1.5391568585381229E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5856789332809158E-2</c:v>
+                  <c:v>9.9999999999374151E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,7 +586,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 4</c:v>
+                  <c:v>State 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -655,43 +655,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.0735624609932321E-2</c:v>
+                  <c:v>2.2047684234645749E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4113077583493553E-2</c:v>
+                  <c:v>1.3046972424085569E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1054355745552197E-2</c:v>
+                  <c:v>4.0629114033052673E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1575702728459232</c:v>
+                  <c:v>7.890445842796287E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.673966584248299E-2</c:v>
+                  <c:v>0.2251178363368572</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60610067961852132</c:v>
+                  <c:v>4.0253851422455973E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60385173341770948</c:v>
+                  <c:v>4.2563427158311944E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0847866992160817E-2</c:v>
+                  <c:v>9.999999999810545E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5846966214778949E-2</c:v>
+                  <c:v>0.74584821953227221</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.2494510671060764E-3</c:v>
+                  <c:v>5.7907677807776448E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.496587641206412E-3</c:v>
+                  <c:v>0.2218930660137203</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5391568585381229E-2</c:v>
+                  <c:v>4.2385023482237487E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.9999999999374151E-11</c:v>
+                  <c:v>0.60238862898699674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -711,7 +711,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 5</c:v>
+                  <c:v>State 7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -780,43 +780,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.649360204415663</c:v>
+                  <c:v>9.9266899788873972E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27031522112167289</c:v>
+                  <c:v>3.2755438962968647E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9697562257589876E-3</c:v>
+                  <c:v>8.8453421207645905E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3136311312309186E-3</c:v>
+                  <c:v>4.4334187684589833E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9775353334575342E-3</c:v>
+                  <c:v>0.82168261428507128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5897686511381843E-3</c:v>
+                  <c:v>1.8021864456828199E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6919380892336781E-2</c:v>
+                  <c:v>0.95570436999934982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.143707225202466E-3</c:v>
+                  <c:v>0.4032438476709943</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13086363748125951</c:v>
+                  <c:v>0.35586835220453489</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6330012126481198E-2</c:v>
+                  <c:v>9.3334541563073678E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9999999998208679E-11</c:v>
+                  <c:v>0.2050057369189798</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.2270231567373227E-3</c:v>
+                  <c:v>0.99999212747904642</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0409090585301309E-3</c:v>
+                  <c:v>0.47770535353306448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -836,7 +836,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 6</c:v>
+                  <c:v>State 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -905,43 +905,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.2625069243399797E-3</c:v>
+                  <c:v>0.21726863326839521</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1583387228885309</c:v>
+                  <c:v>6.2799956205332547E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2360558366148671E-3</c:v>
+                  <c:v>3.8765374118686108E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42079215933093977</c:v>
+                  <c:v>3.860521497585321E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2122018740809969E-2</c:v>
+                  <c:v>3.5165162606031692E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0676260903289369E-2</c:v>
+                  <c:v>3.3155059660385122E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.999999999920666E-11</c:v>
+                  <c:v>9.9999999990087394E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3095388591764453</c:v>
+                  <c:v>0.4262896519754919</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.9074146891717845E-2</c:v>
+                  <c:v>4.6531237197536032E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51097211206557314</c:v>
+                  <c:v>4.9064631494888829E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8331160920852388E-2</c:v>
+                  <c:v>9.9999999992495097E-11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.84011446552460134</c:v>
+                  <c:v>0.15455729869780421</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27125329754273608</c:v>
+                  <c:v>0.14965503018695939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -961,7 +961,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 7</c:v>
+                  <c:v>State 3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1032,43 +1032,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>9.9266899788873972E-2</c:v>
+                  <c:v>0.54070007486828675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2755438962968647E-2</c:v>
+                  <c:v>5.5407104201901702E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.8453421207645905E-2</c:v>
+                  <c:v>0.74504643821964256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4334187684589833E-2</c:v>
+                  <c:v>0.354811901022903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82168261428507128</c:v>
+                  <c:v>0.1161355908351684</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8021864456828199E-2</c:v>
+                  <c:v>0.1395758925812996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.95570436999934982</c:v>
+                  <c:v>4.4365109338377222E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4032438476709943</c:v>
+                  <c:v>1.5199893524897879E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.35586835220453489</c:v>
+                  <c:v>0.1207850320130895</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.3334541563073678E-2</c:v>
+                  <c:v>2.6916553455223549E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2050057369189798</c:v>
+                  <c:v>0.81366235053645242</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99999212747904642</c:v>
+                  <c:v>0.63731989643767506</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.47770535353306448</c:v>
+                  <c:v>1.5856789332809158E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1088,7 +1088,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State 8</c:v>
+                  <c:v>State 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1159,43 +1159,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>9.9999999999321573E-11</c:v>
+                  <c:v>0.649360204415663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7016265604056392</c:v>
+                  <c:v>0.27031522112167289</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42442550141671692</c:v>
+                  <c:v>7.9697562257589876E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45728933537503152</c:v>
+                  <c:v>6.3136311312309186E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3852416398575028E-2</c:v>
+                  <c:v>8.9775353334575342E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35407924289997772</c:v>
+                  <c:v>5.5897686511381843E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6142408067212128E-2</c:v>
+                  <c:v>2.6919380892336781E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77757230967003532</c:v>
+                  <c:v>2.143707225202466E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9356090172584577E-2</c:v>
+                  <c:v>0.13086363748125951</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.89260979170291921</c:v>
+                  <c:v>1.6330012126481198E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74065643991960151</c:v>
+                  <c:v>9.9999999998208679E-11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99755492546134183</c:v>
+                  <c:v>6.2270231567373227E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5692203845545537</c:v>
+                  <c:v>3.0409090585301309E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2316,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2373,359 +2373,364 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>2.2047684234645749E-2</v>
+        <v>9.9999999999321573E-11</v>
       </c>
       <c r="C2">
-        <v>1.3046972424085569E-2</v>
+        <v>0.7016265604056392</v>
       </c>
       <c r="D2">
-        <v>4.0629114033052673E-2</v>
+        <v>0.42442550141671692</v>
       </c>
       <c r="E2">
-        <v>7.890445842796287E-3</v>
+        <v>0.45728933537503152</v>
       </c>
       <c r="F2">
-        <v>0.2251178363368572</v>
+        <v>9.3852416398575028E-2</v>
       </c>
       <c r="G2">
-        <v>4.0253851422455973E-2</v>
+        <v>0.35407924289997772</v>
       </c>
       <c r="H2">
-        <v>4.2563427158311944E-3</v>
+        <v>4.6142408067212128E-2</v>
       </c>
       <c r="I2">
-        <v>9.999999999810545E-11</v>
+        <v>0.77757230967003532</v>
       </c>
       <c r="J2">
-        <v>0.74584821953227221</v>
+        <v>4.9356090172584577E-2</v>
       </c>
       <c r="K2">
-        <v>5.7907677807776448E-2</v>
+        <v>0.89260979170291921</v>
       </c>
       <c r="L2">
-        <v>0.2218930660137203</v>
+        <v>0.74065643991960151</v>
       </c>
       <c r="M2">
-        <v>4.2385023482237487E-2</v>
+        <v>0.99755492546134183</v>
       </c>
       <c r="N2">
-        <v>0.60238862898699674</v>
+        <v>0.5692203845545537</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>0.21726863326839521</v>
+        <v>5.2625069243399797E-3</v>
       </c>
       <c r="C3">
-        <v>6.2799956205332547E-2</v>
+        <v>0.1583387228885309</v>
       </c>
       <c r="D3">
-        <v>3.8765374118686108E-2</v>
+        <v>3.2360558366148671E-3</v>
       </c>
       <c r="E3">
-        <v>3.860521497585321E-3</v>
+        <v>0.42079215933093977</v>
       </c>
       <c r="F3">
-        <v>3.5165162606031692E-3</v>
+        <v>2.2122018740809969E-2</v>
       </c>
       <c r="G3">
-        <v>3.3155059660385122E-2</v>
+        <v>2.0676260903289369E-2</v>
       </c>
       <c r="H3">
-        <v>9.9999999990087394E-11</v>
+        <v>9.999999999920666E-11</v>
       </c>
       <c r="I3">
-        <v>0.4262896519754919</v>
+        <v>0.3095388591764453</v>
       </c>
       <c r="J3">
-        <v>4.6531237197536032E-2</v>
+        <v>8.9074146891717845E-2</v>
       </c>
       <c r="K3">
-        <v>4.9064631494888829E-3</v>
+        <v>0.51097211206557314</v>
       </c>
       <c r="L3">
-        <v>9.9999999992495097E-11</v>
+        <v>2.8331160920852388E-2</v>
       </c>
       <c r="M3">
-        <v>0.15455729869780421</v>
+        <v>0.84011446552460134</v>
       </c>
       <c r="N3">
-        <v>0.14965503018695939</v>
+        <v>0.27125329754273608</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>0.54070007486828675</v>
+        <v>1.0735624609932321E-2</v>
       </c>
       <c r="C4">
-        <v>5.5407104201901702E-2</v>
+        <v>4.4113077583493553E-2</v>
       </c>
       <c r="D4">
-        <v>0.74504643821964256</v>
+        <v>4.1054355745552197E-2</v>
       </c>
       <c r="E4">
-        <v>0.354811901022903</v>
+        <v>0.1575702728459232</v>
       </c>
       <c r="F4">
-        <v>0.1161355908351684</v>
+        <v>1.673966584248299E-2</v>
       </c>
       <c r="G4">
-        <v>0.1395758925812996</v>
+        <v>0.60610067961852132</v>
       </c>
       <c r="H4">
-        <v>4.4365109338377222E-2</v>
+        <v>0.60385173341770948</v>
       </c>
       <c r="I4">
-        <v>1.5199893524897879E-2</v>
+        <v>5.0847866992160817E-2</v>
       </c>
       <c r="J4">
-        <v>0.1207850320130895</v>
+        <v>1.5846966214778949E-2</v>
       </c>
       <c r="K4">
-        <v>2.6916553455223549E-3</v>
+        <v>5.2494510671060764E-3</v>
       </c>
       <c r="L4">
-        <v>0.81366235053645242</v>
+        <v>3.496587641206412E-3</v>
       </c>
       <c r="M4">
-        <v>0.63731989643767506</v>
+        <v>1.5391568585381229E-2</v>
       </c>
       <c r="N4">
-        <v>1.5856789332809158E-2</v>
+        <v>9.9999999999374151E-11</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>1.0735624609932321E-2</v>
+        <v>2.2047684234645749E-2</v>
       </c>
       <c r="C5">
-        <v>4.4113077583493553E-2</v>
+        <v>1.3046972424085569E-2</v>
       </c>
       <c r="D5">
-        <v>4.1054355745552197E-2</v>
+        <v>4.0629114033052673E-2</v>
       </c>
       <c r="E5">
-        <v>0.1575702728459232</v>
+        <v>7.890445842796287E-3</v>
       </c>
       <c r="F5">
-        <v>1.673966584248299E-2</v>
+        <v>0.2251178363368572</v>
       </c>
       <c r="G5">
-        <v>0.60610067961852132</v>
+        <v>4.0253851422455973E-2</v>
       </c>
       <c r="H5">
-        <v>0.60385173341770948</v>
+        <v>4.2563427158311944E-3</v>
       </c>
       <c r="I5">
-        <v>5.0847866992160817E-2</v>
+        <v>9.999999999810545E-11</v>
       </c>
       <c r="J5">
-        <v>1.5846966214778949E-2</v>
+        <v>0.74584821953227221</v>
       </c>
       <c r="K5">
-        <v>5.2494510671060764E-3</v>
+        <v>5.7907677807776448E-2</v>
       </c>
       <c r="L5">
-        <v>3.496587641206412E-3</v>
+        <v>0.2218930660137203</v>
       </c>
       <c r="M5">
-        <v>1.5391568585381229E-2</v>
+        <v>4.2385023482237487E-2</v>
       </c>
       <c r="N5">
-        <v>9.9999999999374151E-11</v>
+        <v>0.60238862898699674</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>0.649360204415663</v>
+        <v>9.9266899788873972E-2</v>
       </c>
       <c r="C6">
-        <v>0.27031522112167289</v>
+        <v>3.2755438962968647E-2</v>
       </c>
       <c r="D6">
-        <v>7.9697562257589876E-3</v>
+        <v>8.8453421207645905E-2</v>
       </c>
       <c r="E6">
-        <v>6.3136311312309186E-3</v>
+        <v>4.4334187684589833E-2</v>
       </c>
       <c r="F6">
-        <v>8.9775353334575342E-3</v>
+        <v>0.82168261428507128</v>
       </c>
       <c r="G6">
-        <v>5.5897686511381843E-3</v>
+        <v>1.8021864456828199E-2</v>
       </c>
       <c r="H6">
-        <v>2.6919380892336781E-2</v>
+        <v>0.95570436999934982</v>
       </c>
       <c r="I6">
-        <v>2.143707225202466E-3</v>
+        <v>0.4032438476709943</v>
       </c>
       <c r="J6">
-        <v>0.13086363748125951</v>
+        <v>0.35586835220453489</v>
       </c>
       <c r="K6">
-        <v>1.6330012126481198E-2</v>
+        <v>9.3334541563073678E-2</v>
       </c>
       <c r="L6">
-        <v>9.9999999998208679E-11</v>
+        <v>0.2050057369189798</v>
       </c>
       <c r="M6">
-        <v>6.2270231567373227E-3</v>
+        <v>0.99999212747904642</v>
       </c>
       <c r="N6">
-        <v>3.0409090585301309E-3</v>
+        <v>0.47770535353306448</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>5.2625069243399797E-3</v>
+        <v>0.21726863326839521</v>
       </c>
       <c r="C7">
-        <v>0.1583387228885309</v>
+        <v>6.2799956205332547E-2</v>
       </c>
       <c r="D7">
-        <v>3.2360558366148671E-3</v>
+        <v>3.8765374118686108E-2</v>
       </c>
       <c r="E7">
-        <v>0.42079215933093977</v>
+        <v>3.860521497585321E-3</v>
       </c>
       <c r="F7">
-        <v>2.2122018740809969E-2</v>
+        <v>3.5165162606031692E-3</v>
       </c>
       <c r="G7">
-        <v>2.0676260903289369E-2</v>
+        <v>3.3155059660385122E-2</v>
       </c>
       <c r="H7">
-        <v>9.999999999920666E-11</v>
+        <v>9.9999999990087394E-11</v>
       </c>
       <c r="I7">
-        <v>0.3095388591764453</v>
+        <v>0.4262896519754919</v>
       </c>
       <c r="J7">
-        <v>8.9074146891717845E-2</v>
+        <v>4.6531237197536032E-2</v>
       </c>
       <c r="K7">
-        <v>0.51097211206557314</v>
+        <v>4.9064631494888829E-3</v>
       </c>
       <c r="L7">
-        <v>2.8331160920852388E-2</v>
+        <v>9.9999999992495097E-11</v>
       </c>
       <c r="M7">
-        <v>0.84011446552460134</v>
+        <v>0.15455729869780421</v>
       </c>
       <c r="N7">
-        <v>0.27125329754273608</v>
+        <v>0.14965503018695939</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>9.9266899788873972E-2</v>
+        <v>0.54070007486828675</v>
       </c>
       <c r="C8">
-        <v>3.2755438962968647E-2</v>
+        <v>5.5407104201901702E-2</v>
       </c>
       <c r="D8">
-        <v>8.8453421207645905E-2</v>
+        <v>0.74504643821964256</v>
       </c>
       <c r="E8">
-        <v>4.4334187684589833E-2</v>
+        <v>0.354811901022903</v>
       </c>
       <c r="F8">
-        <v>0.82168261428507128</v>
+        <v>0.1161355908351684</v>
       </c>
       <c r="G8">
-        <v>1.8021864456828199E-2</v>
+        <v>0.1395758925812996</v>
       </c>
       <c r="H8">
-        <v>0.95570436999934982</v>
+        <v>4.4365109338377222E-2</v>
       </c>
       <c r="I8">
-        <v>0.4032438476709943</v>
+        <v>1.5199893524897879E-2</v>
       </c>
       <c r="J8">
-        <v>0.35586835220453489</v>
+        <v>0.1207850320130895</v>
       </c>
       <c r="K8">
-        <v>9.3334541563073678E-2</v>
+        <v>2.6916553455223549E-3</v>
       </c>
       <c r="L8">
-        <v>0.2050057369189798</v>
+        <v>0.81366235053645242</v>
       </c>
       <c r="M8">
-        <v>0.99999212747904642</v>
+        <v>0.63731989643767506</v>
       </c>
       <c r="N8">
-        <v>0.47770535353306448</v>
+        <v>1.5856789332809158E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>9.9999999999321573E-11</v>
+        <v>0.649360204415663</v>
       </c>
       <c r="C9">
-        <v>0.7016265604056392</v>
+        <v>0.27031522112167289</v>
       </c>
       <c r="D9">
-        <v>0.42442550141671692</v>
+        <v>7.9697562257589876E-3</v>
       </c>
       <c r="E9">
-        <v>0.45728933537503152</v>
+        <v>6.3136311312309186E-3</v>
       </c>
       <c r="F9">
-        <v>9.3852416398575028E-2</v>
+        <v>8.9775353334575342E-3</v>
       </c>
       <c r="G9">
-        <v>0.35407924289997772</v>
+        <v>5.5897686511381843E-3</v>
       </c>
       <c r="H9">
-        <v>4.6142408067212128E-2</v>
+        <v>2.6919380892336781E-2</v>
       </c>
       <c r="I9">
-        <v>0.77757230967003532</v>
+        <v>2.143707225202466E-3</v>
       </c>
       <c r="J9">
-        <v>4.9356090172584577E-2</v>
+        <v>0.13086363748125951</v>
       </c>
       <c r="K9">
-        <v>0.89260979170291921</v>
+        <v>1.6330012126481198E-2</v>
       </c>
       <c r="L9">
-        <v>0.74065643991960151</v>
+        <v>9.9999999998208679E-11</v>
       </c>
       <c r="M9">
-        <v>0.99755492546134183</v>
+        <v>6.2270231567373227E-3</v>
       </c>
       <c r="N9">
-        <v>0.5692203845545537</v>
+        <v>3.0409090585301309E-3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="B2:N9">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2735,6 +2740,14 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>